<commit_message>
Updated spreadsheet for P20 resubmission
</commit_message>
<xml_diff>
--- a/Documents/Dichter-data.xlsx
+++ b/Documents/Dichter-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="520" windowWidth="25600" windowHeight="16060" activeTab="1"/>
+    <workbookView xWindow="6820" yWindow="24140" windowWidth="22520" windowHeight="15440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original Dichter data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="287">
   <si>
     <t>Rat</t>
   </si>
@@ -196,18 +196,6 @@
     <t>R118</t>
   </si>
   <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>Start Time</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
-    <t>End Time</t>
-  </si>
-  <si>
     <t>Rat ID</t>
   </si>
   <si>
@@ -355,15 +343,9 @@
     <t xml:space="preserve">file: r130_021.eeg   start: 10/11/2009 00:00:00   end: 11-Oct-2009 02:59:59 </t>
   </si>
   <si>
-    <t>animal zapped at 49 days by mistake</t>
-  </si>
-  <si>
     <t>I032_A0005</t>
   </si>
   <si>
-    <t>converted only channels 1-6</t>
-  </si>
-  <si>
     <t>I032_A0001</t>
   </si>
   <si>
@@ -739,274 +721,166 @@
     <t xml:space="preserve">file: r137_000.eeg   start: 12/21/2009 16:33:22   end: 21-Dec-2009 17:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_000.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_001.eeg   start: 12/24/2009 12:45:22   end: 24-Dec-2009 14:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_001.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_002.eeg   start: 12/27/2009 00:00:01   end: 27-Dec-2009 03:00:00 </t>
   </si>
   <si>
-    <t>Testing r137_002.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_003.eeg   start: 12/27/2009 15:17:47   end: 27-Dec-2009 17:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_003.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_004.eeg   start: 01/03/2010 00:00:00   end: 03-Jan-2010 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_004.eeg channel 1. PerTesting r137_004.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_005.eeg   start: 01/10/2010 00:00:00   end: 10-Jan-2010 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_005.eeg channel 1. PerTesting r137_005.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_006.eeg   start: 01/15/2010 09:39:27   end: 15-Jan-2010 11:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_006.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_007.eeg   start: 01/17/2010 00:00:00   end: 17-Jan-2010 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_007.eeg channel 1. PerTesting r137_007.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_008.eeg   start: 01/24/2010 00:00:00   end: 24-Jan-2010 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_008.eeg channel 1. PerTesting r137_008.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_009.eeg   start: 01/31/2010 00:00:00   end: 31-Jan-2010 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_009.eeg channel 1. PerTesting r137_009.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_010.eeg   start: 02/07/2010 00:00:00   end: 07-Feb-2010 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_010.eeg channel 1. PerTesting r137_010.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_011.eeg   start: 02/14/2010 00:00:00   end: 14-Feb-2010 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_011.eeg channel 1. PerTesting r137_011.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_012.eeg   start: 02/21/2010 00:00:00   end: 21-Feb-2010 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_012.eeg channel 1. PerTesting r137_012.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_013.eeg   start: 02/22/2010 19:44:18   end: 22-Feb-2010 20:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_013.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_014.eeg   start: 02/28/2010 00:00:00   end: 28-Feb-2010 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_014.eeg channel 1. PerTesting r137_014.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_015.eeg   start: 03/07/2010 00:00:00   end: 07-Mar-2010 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_015.eeg channel 1. PerTesting r137_015.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_016.eeg   start: 03/14/2010 00:00:00   end: 14-Mar-2010 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_016.eeg channel 1. PerTesting r137_016.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r137_017.eeg   start: 03/21/2010 00:00:01   end: 21-Mar-2010 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r137_017.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
-    <t>Elapsed time is 307.570838 seconds.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_000.eeg   start: 03/02/2011 16:15:16   end: 02-Mar-2011 17:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_000.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_001.eeg   start: 03/06/2011 00:00:00   end: 06-Mar-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_001.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_002.eeg   start: 03/13/2011 00:00:00   end: 13-Mar-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_002.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_003.eeg   start: 03/20/2011 00:00:00   end: 20-Mar-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_003.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_004.eeg   start: 03/27/2011 00:00:00   end: 27-Mar-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_004.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_005.eeg   start: 04/03/2011 00:00:00   end: 03-Apr-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_005.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_006.eeg   start: 04/07/2011 13:04:45   end: 07-Apr-2011 14:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_006.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_007.eeg   start: 04/10/2011 00:00:00   end: 10-Apr-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_007.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_008.eeg   start: 04/12/2011 12:33:59   end: 12-Apr-2011 14:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_008.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_009.eeg   start: 04/17/2011 00:00:00   end: 17-Apr-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_009.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_010.eeg   start: 04/20/2011 08:41:22   end: 20-Apr-2011 08:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_010.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_011.eeg   start: 04/24/2011 00:00:00   end: 24-Apr-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_011.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r151_012.eeg   start: 05/01/2011 00:00:00   end: 01-May-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r151_012.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
-    <t>Disregarding r151_ch1_SeizureData.eeg</t>
-  </si>
-  <si>
-    <t>Elapsed time is 568.300767 seconds.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r152_000.eeg   start: 04/12/2011 12:33:59   end: 12-Apr-2011 14:59:59 </t>
   </si>
   <si>
-    <t>Testing r152_000.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r152_001.eeg   start: 04/17/2011 00:00:00   end: 17-Apr-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r152_001.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r152_002.eeg   start: 04/20/2011 08:41:22   end: 20-Apr-2011 08:59:59 </t>
   </si>
   <si>
-    <t>Testing r152_002.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r152_003.eeg   start: 04/24/2011 00:00:00   end: 24-Apr-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r152_003.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r152_004.eeg   start: 05/01/2011 00:00:00   end: 01-May-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r152_004.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r152_005.eeg   start: 05/04/2011 20:03:45   end: 04-May-2011 20:59:59 </t>
   </si>
   <si>
-    <t>Testing r152_005.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r152_006.eeg   start: 05/08/2011 00:00:00   end: 08-May-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r152_006.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r152_007.eeg   start: 05/15/2011 00:00:00   end: 15-May-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r152_007.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r152_008.eeg   start: 05/17/2011 08:27:27   end: 17-May-2011 08:59:59 </t>
   </si>
   <si>
-    <t>Testing r152_008.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r152_009.eeg   start: 05/22/2011 00:00:00   end: 22-May-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r152_009.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r152_010.eeg   start: 05/29/2011 00:00:00   end: 29-May-2011 02:59:59 </t>
   </si>
   <si>
-    <t>Testing r152_010.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
     <t xml:space="preserve">file: r152_011.eeg   start: 06/02/2011 09:13:40   end: 02-Jun-2011 11:59:59 </t>
   </si>
   <si>
-    <t>Testing r152_011.eeg channel 1. Percent finished: 100.0.</t>
-  </si>
-  <si>
-    <t>Disregarding r152_ch1_SeizureData.eeg</t>
-  </si>
-  <si>
-    <t>Elapsed time is 775.724671 seconds.</t>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Recording Times</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>-, converted only channels 1-6</t>
+  </si>
+  <si>
+    <t>Days of Recording</t>
+  </si>
+  <si>
+    <t>Control Days</t>
+  </si>
+  <si>
+    <t>Seizures?</t>
+  </si>
+  <si>
+    <t>Uploaded</t>
+  </si>
+  <si>
+    <t>Converted</t>
+  </si>
+  <si>
+    <t>Analyzed</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1036,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="171">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1334,8 +1208,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1436,7 +1338,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1448,14 +1349,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="171">
+  <cellStyles count="199">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1541,6 +1468,20 @@
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1626,6 +1567,20 @@
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1928,10 +1883,10 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:C48"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3022,183 +2977,227 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O326"/>
+  <dimension ref="A2:P190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F125" workbookViewId="0">
-      <selection activeCell="K146" sqref="K146"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.5" style="35" customWidth="1"/>
     <col min="2" max="3" width="15.83203125" style="35" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="35" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="35"/>
-    <col min="7" max="7" width="16.6640625" style="35" customWidth="1"/>
-    <col min="8" max="9" width="15.83203125" style="35" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" style="35"/>
-    <col min="12" max="12" width="24.6640625" style="35" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="35" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="35" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="35"/>
+    <col min="4" max="4" width="5.6640625" style="35" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="35" customWidth="1"/>
+    <col min="6" max="8" width="10.83203125" style="35"/>
+    <col min="9" max="9" width="16.6640625" style="35" customWidth="1"/>
+    <col min="10" max="11" width="15.83203125" style="35" customWidth="1"/>
+    <col min="12" max="14" width="10.83203125" style="35"/>
+    <col min="15" max="15" width="60.6640625" style="35" customWidth="1"/>
+    <col min="16" max="18" width="20" style="35" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="35"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="13" thickBot="1"/>
-    <row r="3" spans="1:15" ht="33" thickBot="1">
-      <c r="A3" s="47" t="s">
+    <row r="2" spans="1:16" ht="13" thickBot="1"/>
+    <row r="3" spans="1:16" ht="49" thickBot="1">
+      <c r="A3" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3"/>
+      <c r="C3" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="46"/>
       <c r="E3" s="34" t="s">
-        <v>62</v>
+        <v>275</v>
       </c>
       <c r="F3" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="42" t="s">
-        <v>160</v>
-      </c>
-      <c r="K3" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="42" t="s">
+      <c r="H3" s="53" t="s">
+        <v>280</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>281</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>282</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>284</v>
+      </c>
+      <c r="L3" s="60" t="s">
+        <v>283</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="O3" s="41" t="s">
+        <v>276</v>
+      </c>
+      <c r="P3" s="42" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="13" thickBot="1">
+      <c r="A4" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="18">
+        <v>1</v>
+      </c>
+      <c r="F4" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="M3" s="41" t="s">
+      <c r="G4" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="54">
+        <v>65</v>
+      </c>
+      <c r="I4" s="55">
+        <v>7</v>
+      </c>
+      <c r="J4" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="O4" s="47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="13" thickBot="1">
+      <c r="A5" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="35">
+        <v>2</v>
+      </c>
+      <c r="F5" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="N3" s="42" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="13" thickBot="1">
-      <c r="A4" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" s="18">
-        <v>1</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="G4" s="8">
-        <v>39519</v>
-      </c>
-      <c r="H4" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="K4" s="48" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="13" thickBot="1">
-      <c r="A5" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="35">
-        <v>2</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="G5" s="8">
-        <v>39587</v>
-      </c>
-      <c r="H5" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="K5" s="49" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="G5" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="54">
+        <v>56</v>
+      </c>
+      <c r="I5" s="55">
+        <v>10</v>
+      </c>
+      <c r="J5" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="K5" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="L5" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="M5" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="O5" s="48" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="37" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C6" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="37"/>
+      <c r="E6" s="35">
         <v>3</v>
       </c>
-      <c r="E6" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="G6" s="11">
-        <v>39597</v>
-      </c>
-      <c r="H6" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="K6" s="48" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="F6" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="H6" s="56">
+        <v>53</v>
+      </c>
+      <c r="I6" s="57">
+        <v>7</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="K6" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="L6" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="M6" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="O6" s="47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="37" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B7" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" s="38">
+      <c r="C7" s="61" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38">
         <v>4</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="G7" s="11">
-        <v>39629</v>
-      </c>
-      <c r="H7" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="K7" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="O7" s="8">
+      <c r="F7" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="56">
+        <v>56</v>
+      </c>
+      <c r="I7" s="57">
+        <v>25</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="O7" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="P7" s="8">
         <v>39519</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" s="37" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B8" s="35" t="s">
         <v>47</v>
@@ -3206,1425 +3205,1901 @@
       <c r="C8" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="38">
+      <c r="E8" s="38">
         <v>5</v>
       </c>
-      <c r="E8" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="G8" s="11">
-        <v>39703</v>
-      </c>
-      <c r="H8" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="I8" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="K8" s="35" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="F8" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" s="56">
+        <v>49</v>
+      </c>
+      <c r="I8" s="57">
+        <v>14</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="O8" s="35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="40"/>
+      <c r="E9" s="38">
         <v>6</v>
       </c>
-      <c r="E9" s="38" t="s">
-        <v>68</v>
-      </c>
       <c r="F9" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="G9" s="8">
-        <v>39896</v>
-      </c>
-      <c r="H9" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="K9" s="35" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <v>64</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="56">
+        <v>39</v>
+      </c>
+      <c r="I9" s="55">
+        <v>7</v>
+      </c>
+      <c r="J9" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="K9" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="L9" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="M9" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="O9" s="35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="C10" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="38">
+      <c r="E10" s="38">
         <v>7</v>
       </c>
-      <c r="E10" s="38" t="s">
-        <v>71</v>
-      </c>
       <c r="F10" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="G10" s="11">
-        <v>40036</v>
-      </c>
-      <c r="H10" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="K10" s="35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <v>67</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" s="56">
+        <v>130</v>
+      </c>
+      <c r="I10" s="57">
+        <v>36</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="K10" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="O10" s="35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="39"/>
-      <c r="C11" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="D11" s="38">
+      <c r="C11" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38">
         <v>8</v>
       </c>
-      <c r="E11" s="38" t="s">
-        <v>69</v>
-      </c>
       <c r="F11" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="G11" s="8">
-        <v>40039</v>
-      </c>
-      <c r="H11" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="I11" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="K11" s="35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+        <v>65</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" s="56">
+        <v>159</v>
+      </c>
+      <c r="I11" s="55">
+        <v>24</v>
+      </c>
+      <c r="J11" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="K11" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="O11" s="35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="C12" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="38">
+      <c r="E12" s="38">
         <v>9</v>
       </c>
-      <c r="E12" s="38" t="s">
-        <v>72</v>
-      </c>
       <c r="F12" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="G12" s="11">
-        <v>40192</v>
-      </c>
-      <c r="H12" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="K12" s="35" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+        <v>68</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="H12" s="56">
+        <v>91</v>
+      </c>
+      <c r="I12" s="57">
+        <v>24</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="K12" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="O12" s="35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="37" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="38">
+      <c r="E13" s="38">
         <v>10</v>
       </c>
-      <c r="E13" s="38" t="s">
-        <v>70</v>
-      </c>
       <c r="F13" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" s="22">
-        <v>40618</v>
-      </c>
-      <c r="H13" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="K13" s="35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>66</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="56">
+        <v>63</v>
+      </c>
+      <c r="I13" s="58">
+        <v>14</v>
+      </c>
+      <c r="J13" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="O13" s="35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="37" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="39"/>
+      <c r="E14" s="38">
         <v>11</v>
       </c>
-      <c r="E14" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="F14" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H14" s="59">
+        <v>51</v>
+      </c>
+      <c r="I14" s="58">
+        <v>14</v>
+      </c>
+      <c r="J14" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="O14" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="C15" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="O15" s="35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="O16" s="35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="O17" s="35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="O18" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="P18" s="44"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="P19" s="45"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="O20" s="47" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="P21" s="8">
+        <v>39587</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="35" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="7">
+        <v>97</v>
+      </c>
+      <c r="B24" s="8">
+        <v>39512</v>
+      </c>
+      <c r="C24" s="8">
+        <v>39519</v>
+      </c>
+      <c r="D24" s="8">
+        <v>39577</v>
+      </c>
+      <c r="E24" s="9">
+        <f>D24-B24</f>
+        <v>65</v>
+      </c>
+      <c r="F24" s="9">
+        <f>C24-B24</f>
+        <v>7</v>
+      </c>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="7">
+        <v>99</v>
+      </c>
+      <c r="B26" s="8">
+        <v>39577</v>
+      </c>
+      <c r="C26" s="8">
+        <v>39587</v>
+      </c>
+      <c r="D26" s="8">
+        <v>39633</v>
+      </c>
+      <c r="E26" s="9">
+        <f>D26-B26</f>
+        <v>56</v>
+      </c>
+      <c r="F26" s="9">
+        <f>C26-B26</f>
+        <v>10</v>
+      </c>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28">
+        <v>100</v>
+      </c>
+      <c r="B28" s="11">
+        <v>39590</v>
+      </c>
+      <c r="C28" s="11">
+        <v>39597</v>
+      </c>
+      <c r="D28" s="11">
+        <v>39643</v>
+      </c>
+      <c r="E28" s="2">
+        <f>D28-B28</f>
+        <v>53</v>
+      </c>
+      <c r="F28" s="2">
+        <f>C28-B28</f>
+        <v>7</v>
+      </c>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30">
+        <v>101</v>
+      </c>
+      <c r="B30" s="11">
+        <v>39604</v>
+      </c>
+      <c r="C30" s="11">
+        <v>39629</v>
+      </c>
+      <c r="D30" s="11">
+        <v>39660</v>
+      </c>
+      <c r="E30" s="2">
+        <f>D30-B30</f>
+        <v>56</v>
+      </c>
+      <c r="F30" s="2">
+        <f>C30-B30</f>
+        <v>25</v>
+      </c>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="35" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32">
+        <v>103</v>
+      </c>
+      <c r="B32" s="11">
+        <v>39660</v>
+      </c>
+      <c r="C32" s="11">
+        <v>39675</v>
+      </c>
+      <c r="D32" s="11">
+        <v>39675</v>
+      </c>
+      <c r="E32" s="2">
+        <f>D32-B32</f>
+        <v>15</v>
+      </c>
+      <c r="F32" s="2">
+        <f>C32-B32</f>
+        <v>15</v>
+      </c>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="50"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="47" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="P33" s="52">
+        <v>39597</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="7">
+        <v>104</v>
+      </c>
+      <c r="B34" s="8">
+        <v>39667</v>
+      </c>
+      <c r="C34" s="8">
+        <v>39675</v>
+      </c>
+      <c r="D34" s="8">
+        <v>39870</v>
+      </c>
+      <c r="E34" s="9">
+        <f>D34-B34</f>
+        <v>203</v>
+      </c>
+      <c r="F34" s="9">
+        <f>C34-B34</f>
+        <v>8</v>
+      </c>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="50"/>
+      <c r="N34" s="50"/>
+      <c r="O34" s="35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36">
+        <v>107</v>
+      </c>
+      <c r="B36" s="11">
+        <v>39689</v>
+      </c>
+      <c r="C36" s="11">
+        <v>39703</v>
+      </c>
+      <c r="D36" s="11">
+        <v>39738</v>
+      </c>
+      <c r="E36" s="2">
+        <f>D36-B36</f>
+        <v>49</v>
+      </c>
+      <c r="F36" s="2">
+        <f>C36-B36</f>
+        <v>14</v>
+      </c>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38">
         <v>118</v>
       </c>
-      <c r="G14" s="22">
+      <c r="B38" s="11">
+        <v>39853</v>
+      </c>
+      <c r="C38" s="11">
+        <v>39871</v>
+      </c>
+      <c r="D38" s="11">
+        <v>401461</v>
+      </c>
+      <c r="E38" s="2">
+        <v>18</v>
+      </c>
+      <c r="F38" s="14">
+        <f>C38-B38</f>
+        <v>18</v>
+      </c>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="14"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" s="7">
+        <v>121</v>
+      </c>
+      <c r="B40" s="8">
+        <v>39889</v>
+      </c>
+      <c r="C40" s="8">
+        <v>39896</v>
+      </c>
+      <c r="D40" s="8">
+        <v>39928</v>
+      </c>
+      <c r="E40" s="9">
+        <f>D40-B40</f>
+        <v>39</v>
+      </c>
+      <c r="F40" s="14">
+        <f>C40-B40</f>
+        <v>7</v>
+      </c>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="50"/>
+      <c r="M40" s="50"/>
+      <c r="N40" s="50"/>
+      <c r="O40" s="35" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="49"/>
+      <c r="O41" s="35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42">
+        <v>127</v>
+      </c>
+      <c r="B42" s="11">
+        <v>40000</v>
+      </c>
+      <c r="C42" s="11">
+        <v>40036</v>
+      </c>
+      <c r="D42" s="11">
+        <v>40130</v>
+      </c>
+      <c r="E42" s="14">
+        <f>D42-B42</f>
+        <v>130</v>
+      </c>
+      <c r="F42" s="14">
+        <f>C42-B42</f>
+        <v>36</v>
+      </c>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="50"/>
+      <c r="M42" s="50"/>
+      <c r="N42" s="50"/>
+      <c r="O42" s="35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="49"/>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" s="7">
+        <v>130</v>
+      </c>
+      <c r="B44" s="8">
+        <v>40015</v>
+      </c>
+      <c r="C44" s="8">
+        <v>40039</v>
+      </c>
+      <c r="D44" s="8">
+        <v>40174</v>
+      </c>
+      <c r="E44" s="9">
+        <f>D44-B44</f>
+        <v>159</v>
+      </c>
+      <c r="F44" s="14">
+        <f>C44-B44</f>
+        <v>24</v>
+      </c>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="49"/>
+      <c r="O44" s="47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="49"/>
+      <c r="O45" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="P45" s="11"/>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46">
+        <v>137</v>
+      </c>
+      <c r="B46" s="11">
+        <v>40168</v>
+      </c>
+      <c r="C46" s="11">
+        <v>40192</v>
+      </c>
+      <c r="D46" s="11">
+        <v>40259</v>
+      </c>
+      <c r="E46" s="14">
+        <f>D46-B46</f>
+        <v>91</v>
+      </c>
+      <c r="F46" s="14">
+        <f>C46-B46</f>
+        <v>24</v>
+      </c>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="50"/>
+      <c r="M46" s="50"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="49"/>
+      <c r="M47" s="49"/>
+      <c r="N47" s="49"/>
+      <c r="O47" s="47" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="21">
+        <v>146</v>
+      </c>
+      <c r="B48" s="22">
+        <v>40512</v>
+      </c>
+      <c r="C48" s="22">
+        <v>40547</v>
+      </c>
+      <c r="D48" s="22">
+        <v>40696</v>
+      </c>
+      <c r="E48" s="23">
+        <f>D48-B48</f>
+        <v>184</v>
+      </c>
+      <c r="F48" s="23">
+        <f>C48-B48</f>
+        <v>35</v>
+      </c>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="49"/>
+      <c r="M48" s="49"/>
+      <c r="N48" s="49"/>
+      <c r="O48" s="47" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="49"/>
+      <c r="M49" s="49"/>
+      <c r="N49" s="49"/>
+      <c r="O49" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="P49" s="49">
+        <v>39629</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" s="21">
+        <v>151</v>
+      </c>
+      <c r="B50" s="22">
+        <v>40604</v>
+      </c>
+      <c r="C50" s="22">
+        <v>40618</v>
+      </c>
+      <c r="D50" s="22">
+        <v>40667</v>
+      </c>
+      <c r="E50" s="23">
+        <f>D50-B50</f>
+        <v>63</v>
+      </c>
+      <c r="F50" s="23">
+        <f>C50-B50</f>
+        <v>14</v>
+      </c>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="50"/>
+      <c r="M50" s="50"/>
+      <c r="N50" s="50"/>
+      <c r="O50" s="35" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="49"/>
+      <c r="M51" s="49"/>
+      <c r="N51" s="49"/>
+      <c r="O51" s="35" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" s="21">
+        <v>152</v>
+      </c>
+      <c r="B52" s="22">
+        <v>40645</v>
+      </c>
+      <c r="C52" s="22">
         <v>40659</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="D52" s="22">
+        <v>40696</v>
+      </c>
+      <c r="E52" s="23">
+        <f>D52-B52</f>
+        <v>51</v>
+      </c>
+      <c r="F52" s="23">
+        <f>C52-B52</f>
+        <v>14</v>
+      </c>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="50"/>
+      <c r="M52" s="50"/>
+      <c r="N52" s="50"/>
+      <c r="O52" s="35" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="49"/>
+      <c r="M53" s="49"/>
+      <c r="N53" s="49"/>
+      <c r="O53" s="35" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="11">
+        <v>40680</v>
+      </c>
+      <c r="C54" s="11">
+        <v>40687</v>
+      </c>
+      <c r="D54" s="11">
+        <v>40700</v>
+      </c>
+      <c r="E54" s="14">
+        <f>D54-B54</f>
+        <v>20</v>
+      </c>
+      <c r="F54" s="14">
+        <f>C54-B54</f>
+        <v>7</v>
+      </c>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="50"/>
+      <c r="M54" s="50"/>
+      <c r="N54" s="50"/>
+      <c r="O54" s="35" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="49"/>
+      <c r="M55" s="49"/>
+      <c r="N55" s="49"/>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56">
+        <v>157</v>
+      </c>
+      <c r="B56" s="11">
+        <v>40735</v>
+      </c>
+      <c r="C56" s="11">
+        <v>40743</v>
+      </c>
+      <c r="D56" s="11">
+        <v>40833</v>
+      </c>
+      <c r="E56" s="14">
+        <f>D56-B56</f>
+        <v>98</v>
+      </c>
+      <c r="F56" s="14">
+        <f>C56-B56</f>
+        <v>8</v>
+      </c>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="49"/>
+      <c r="M56" s="49"/>
+      <c r="N56" s="49"/>
+      <c r="O56" s="47" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="49"/>
+      <c r="M57" s="49"/>
+      <c r="N57" s="49"/>
+      <c r="O57" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="P57" s="49">
+        <v>39703</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58">
+        <v>158</v>
+      </c>
+      <c r="B58" s="11">
+        <v>40735</v>
+      </c>
+      <c r="C58" s="11">
+        <v>40743</v>
+      </c>
+      <c r="D58" s="11">
+        <v>40756</v>
+      </c>
+      <c r="E58" s="14">
+        <f>D58-B58</f>
+        <v>21</v>
+      </c>
+      <c r="F58" s="14">
+        <f>C58-B58</f>
+        <v>8</v>
+      </c>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="50"/>
+      <c r="M58" s="50"/>
+      <c r="N58" s="50"/>
+      <c r="O58" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="P58" s="11"/>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="49"/>
+      <c r="M59" s="49"/>
+      <c r="N59" s="49"/>
+      <c r="O59" s="35" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
+      <c r="A60" s="21">
+        <v>161</v>
+      </c>
+      <c r="B60" s="22">
+        <v>40745</v>
+      </c>
+      <c r="C60" s="22">
+        <v>40759</v>
+      </c>
+      <c r="D60" s="22">
+        <v>40794</v>
+      </c>
+      <c r="E60" s="23">
+        <f>D60-B60</f>
+        <v>49</v>
+      </c>
+      <c r="F60" s="23">
+        <f>C60-B60</f>
+        <v>14</v>
+      </c>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="50"/>
+      <c r="M60" s="50"/>
+      <c r="N60" s="50"/>
+      <c r="O60" s="35" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
+      <c r="A61"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="49"/>
+      <c r="M61" s="49"/>
+      <c r="N61" s="49"/>
+      <c r="O61" s="35" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="A62">
+        <v>162</v>
+      </c>
+      <c r="B62" s="11">
+        <v>40752</v>
+      </c>
+      <c r="C62" s="11">
+        <v>40759</v>
+      </c>
+      <c r="D62" s="11">
+        <v>40778</v>
+      </c>
+      <c r="E62" s="14">
+        <f>D62-B62</f>
+        <v>26</v>
+      </c>
+      <c r="F62" s="14">
+        <f>C62-B62</f>
+        <v>7</v>
+      </c>
+      <c r="J62" s="18"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="50"/>
+      <c r="M62" s="50"/>
+      <c r="N62" s="50"/>
+      <c r="O62" s="35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
+      <c r="A63"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="49"/>
+      <c r="M63" s="49"/>
+      <c r="N63" s="49"/>
+      <c r="O63" s="35" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="A64">
+        <v>164</v>
+      </c>
+      <c r="B64" s="11">
+        <v>40778</v>
+      </c>
+      <c r="C64" s="11">
+        <v>40793</v>
+      </c>
+      <c r="D64" s="11">
+        <v>40799</v>
+      </c>
+      <c r="E64" s="14">
+        <f>D64-B64</f>
+        <v>21</v>
+      </c>
+      <c r="F64" s="14">
+        <f>C64-B64</f>
+        <v>15</v>
+      </c>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="50"/>
+      <c r="M64" s="50"/>
+      <c r="N64" s="50"/>
+      <c r="O64" s="35" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
+      <c r="A65"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="49"/>
+      <c r="M65" s="49"/>
+      <c r="N65" s="49"/>
+    </row>
+    <row r="66" spans="1:16">
+      <c r="A66" s="21">
+        <v>165</v>
+      </c>
+      <c r="B66" s="22">
+        <v>40774</v>
+      </c>
+      <c r="C66" s="22">
+        <v>40793</v>
+      </c>
+      <c r="D66" s="22">
+        <v>40857</v>
+      </c>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23">
+        <f>C66-B66</f>
+        <v>19</v>
+      </c>
+      <c r="O66" s="47" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
+      <c r="A67"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="O67" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="P67" s="51">
+        <v>39896</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
+      <c r="A68">
+        <v>168</v>
+      </c>
+      <c r="B68" s="11">
+        <v>40792</v>
+      </c>
+      <c r="C68" s="11">
+        <v>40798</v>
+      </c>
+      <c r="D68" s="11">
+        <v>40843</v>
+      </c>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14">
+        <f>C68-B68</f>
+        <v>6</v>
+      </c>
+      <c r="O68" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="P68" s="49"/>
+    </row>
+    <row r="69" spans="1:16">
+      <c r="O69" s="35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
+      <c r="O70" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="K14" s="35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="C15" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" s="35" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="K16" s="35" t="s">
+    </row>
+    <row r="71" spans="1:16">
+      <c r="O71" s="35" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
+      <c r="O72" s="35" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
+      <c r="O73" s="35" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
+      <c r="O74" s="35" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
+      <c r="O75" s="35" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
+      <c r="O77" s="47" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16">
+      <c r="O78" s="47" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16">
+      <c r="O79" s="47" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
+      <c r="O80" s="47" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="15:16">
+      <c r="O81" s="47" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="82" spans="15:16">
+      <c r="O82" s="47" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="83" spans="15:16">
+      <c r="O83" s="47" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="84" spans="15:16">
+      <c r="O84" s="47" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="85" spans="15:16">
+      <c r="O85" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="P85" s="11">
+        <v>40036</v>
+      </c>
+    </row>
+    <row r="86" spans="15:16">
+      <c r="O86" s="35" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="87" spans="15:16">
+      <c r="O87" s="35" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="88" spans="15:16">
+      <c r="O88" s="35" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="89" spans="15:16">
+      <c r="O89" s="35" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="90" spans="15:16">
+      <c r="O90" s="35" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="91" spans="15:16">
+      <c r="O91" s="35" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="92" spans="15:16">
+      <c r="O92" s="35" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="93" spans="15:16">
+      <c r="O93" s="35" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="94" spans="15:16">
+      <c r="O94" s="35" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="95" spans="15:16">
+      <c r="O95" s="35" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="96" spans="15:16">
+      <c r="O96" s="35" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="97" spans="15:15">
+      <c r="O97" s="35" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="98" spans="15:15">
+      <c r="O98" s="35" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="99" spans="15:15">
+      <c r="O99" s="35" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="100" spans="15:15">
+      <c r="O100" s="35" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="101" spans="15:15">
+      <c r="O101" s="35" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="102" spans="15:15">
+      <c r="O102" s="35" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="103" spans="15:15">
+      <c r="O103" s="35" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="104" spans="15:15">
+      <c r="O104" s="35" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="105" spans="15:15">
+      <c r="O105" s="35" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="107" spans="15:15">
+      <c r="O107" s="47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="108" spans="15:15">
+      <c r="O108" s="47" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="8:15">
-      <c r="K17" s="35" t="s">
+    <row r="109" spans="15:15">
+      <c r="O109" s="47" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="8:15">
-      <c r="K18" s="35" t="s">
+    <row r="110" spans="15:15">
+      <c r="O110" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="M18" s="38"/>
-      <c r="O18" s="45"/>
-    </row>
-    <row r="19" spans="8:15">
-      <c r="M19" s="38"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="46"/>
-    </row>
-    <row r="20" spans="8:15">
-      <c r="K20" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="N20" s="44"/>
-    </row>
-    <row r="21" spans="8:15">
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="O21" s="8">
-        <v>39587</v>
-      </c>
-    </row>
-    <row r="22" spans="8:15">
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="35" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="8:15">
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="8:15">
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="35" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="8:15">
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="35" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="8:15">
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="35" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="8:15">
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="35" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="28" spans="8:15">
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="35" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="8:15">
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="35" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="8:15">
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="35" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="8:15">
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="50"/>
-    </row>
-    <row r="32" spans="8:15">
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="51"/>
-      <c r="K32" s="48" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="8:15">
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="50"/>
-      <c r="K33" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="O33" s="52">
-        <v>39597</v>
-      </c>
-    </row>
-    <row r="34" spans="8:15">
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="35" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="8:15">
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="35" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="8:15">
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="35" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="8:15">
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="8:15">
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="51"/>
-      <c r="K38" s="35" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="8:15">
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="50"/>
-      <c r="K39" s="35" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="40" spans="8:15">
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="35" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="8:15">
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="50"/>
-      <c r="K41" s="35" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="8:15">
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="51"/>
-      <c r="K42" s="35" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="8:15">
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="50"/>
-    </row>
-    <row r="44" spans="8:15">
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="50"/>
-      <c r="K44" s="48" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="45" spans="8:15">
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="50"/>
-      <c r="K45" s="48" t="s">
-        <v>162</v>
-      </c>
-      <c r="O45" s="11"/>
-    </row>
-    <row r="46" spans="8:15">
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="51"/>
-      <c r="K46" s="48" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="47" spans="8:15">
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="50"/>
-      <c r="K47" s="48" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="48" spans="8:15">
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="50"/>
-      <c r="K48" s="48" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="49" spans="8:15">
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="50"/>
-      <c r="K49" s="48" t="s">
-        <v>166</v>
-      </c>
-      <c r="O49" s="22">
-        <v>39629</v>
-      </c>
-    </row>
-    <row r="50" spans="8:15">
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="51"/>
-      <c r="K50" s="35" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="8:15">
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="50"/>
-      <c r="K51" s="35" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="52" spans="8:15">
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="51"/>
-      <c r="K52" s="35" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="53" spans="8:15">
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="50"/>
-      <c r="K53" s="35" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="54" spans="8:15">
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="51"/>
-      <c r="K54" s="35" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="55" spans="8:15">
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="50"/>
-    </row>
-    <row r="56" spans="8:15">
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="50"/>
-      <c r="K56" s="48" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="57" spans="8:15">
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="50"/>
-      <c r="K57" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="O57" s="22">
-        <v>39703</v>
-      </c>
-    </row>
-    <row r="58" spans="8:15">
-      <c r="H58" s="18"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="51"/>
-      <c r="K58" s="35" t="s">
-        <v>174</v>
-      </c>
-      <c r="O58" s="11"/>
-    </row>
-    <row r="59" spans="8:15">
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
-      <c r="J59" s="50"/>
-      <c r="K59" s="35" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="60" spans="8:15">
-      <c r="H60" s="18"/>
-      <c r="I60" s="18"/>
-      <c r="J60" s="51"/>
-      <c r="K60" s="35" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="61" spans="8:15">
-      <c r="H61" s="18"/>
-      <c r="I61" s="18"/>
-      <c r="J61" s="50"/>
-      <c r="K61" s="35" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="62" spans="8:15">
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
-      <c r="J62" s="51"/>
-      <c r="K62" s="35" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="63" spans="8:15">
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="50"/>
-      <c r="K63" s="35" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="64" spans="8:15">
-      <c r="H64" s="18"/>
-      <c r="I64" s="18"/>
-      <c r="J64" s="51"/>
-      <c r="K64" s="35" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="65" spans="8:15">
-      <c r="H65" s="18"/>
-      <c r="I65" s="18"/>
-      <c r="J65" s="50"/>
-    </row>
-    <row r="66" spans="8:15">
-      <c r="K66" s="48" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="67" spans="8:15">
-      <c r="K67" s="48" t="s">
-        <v>184</v>
-      </c>
-      <c r="O67" s="53">
-        <v>39896</v>
-      </c>
-    </row>
-    <row r="68" spans="8:15">
-      <c r="K68" s="35" t="s">
-        <v>185</v>
-      </c>
-      <c r="O68" s="50"/>
-    </row>
-    <row r="69" spans="8:15">
-      <c r="K69" s="35" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="70" spans="8:15">
-      <c r="K70" s="35" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="71" spans="8:15">
-      <c r="K71" s="35" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="72" spans="8:15">
-      <c r="K72" s="35" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="73" spans="8:15">
-      <c r="K73" s="35" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="74" spans="8:15">
-      <c r="K74" s="35" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="75" spans="8:15">
-      <c r="K75" s="35" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="77" spans="8:15">
-      <c r="K77" s="48" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="78" spans="8:15">
-      <c r="K78" s="48" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="79" spans="8:15">
-      <c r="K79" s="48" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="80" spans="8:15">
-      <c r="K80" s="48" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="81" spans="11:15">
-      <c r="K81" s="48" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="82" spans="11:15">
-      <c r="K82" s="48" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="83" spans="11:15">
-      <c r="K83" s="48" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="84" spans="11:15">
-      <c r="K84" s="48" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="85" spans="11:15">
-      <c r="K85" s="48" t="s">
-        <v>201</v>
-      </c>
-      <c r="O85" s="11">
-        <v>40036</v>
-      </c>
-    </row>
-    <row r="86" spans="11:15">
-      <c r="K86" s="35" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="87" spans="11:15">
-      <c r="K87" s="35" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="88" spans="11:15">
-      <c r="K88" s="35" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="89" spans="11:15">
-      <c r="K89" s="35" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="90" spans="11:15">
-      <c r="K90" s="35" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="91" spans="11:15">
-      <c r="K91" s="35" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="92" spans="11:15">
-      <c r="K92" s="35" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="93" spans="11:15">
-      <c r="K93" s="35" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="94" spans="11:15">
-      <c r="K94" s="35" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="95" spans="11:15">
-      <c r="K95" s="35" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="96" spans="11:15">
-      <c r="K96" s="35" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="97" spans="11:11">
-      <c r="K97" s="35" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="98" spans="11:11">
-      <c r="K98" s="35" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="99" spans="11:11">
-      <c r="K99" s="35" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="100" spans="11:11">
-      <c r="K100" s="35" t="s">
+    </row>
+    <row r="111" spans="15:15">
+      <c r="O111" s="47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="112" spans="15:15">
+      <c r="O112" s="47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="113" spans="15:16">
+      <c r="O113" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="P113" s="8">
+        <v>40039</v>
+      </c>
+    </row>
+    <row r="114" spans="15:16">
+      <c r="O114" s="35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="115" spans="15:16">
+      <c r="O115" s="35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="116" spans="15:16">
+      <c r="O116" s="35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="117" spans="15:16">
+      <c r="O117" s="35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="118" spans="15:16">
+      <c r="O118" s="35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="119" spans="15:16">
+      <c r="O119" s="35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="120" spans="15:16">
+      <c r="O120" s="35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="121" spans="15:16">
+      <c r="O121" s="35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="122" spans="15:16">
+      <c r="O122" s="35" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="123" spans="15:16">
+      <c r="O123" s="35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="124" spans="15:16">
+      <c r="O124" s="35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="15:16">
+      <c r="O125" s="35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="126" spans="15:16">
+      <c r="O126" s="35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="127" spans="15:16">
+      <c r="O127" s="35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="128" spans="15:16">
+      <c r="O128" s="35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="129" spans="15:15">
+      <c r="O129" s="35" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="101" spans="11:11">
-      <c r="K101" s="35" t="s">
+    <row r="130" spans="15:15">
+      <c r="O130" s="35" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="102" spans="11:11">
-      <c r="K102" s="35" t="s">
+    <row r="131" spans="15:15">
+      <c r="O131" s="35" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="103" spans="11:11">
-      <c r="K103" s="35" t="s">
+    <row r="132" spans="15:15">
+      <c r="O132" s="35" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="104" spans="11:11">
-      <c r="K104" s="35" t="s">
+    <row r="133" spans="15:15">
+      <c r="O133" s="35" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="105" spans="11:11">
-      <c r="K105" s="35" t="s">
+    <row r="134" spans="15:15">
+      <c r="O134" s="35" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="107" spans="11:11">
-      <c r="K107" s="48" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="108" spans="11:11">
-      <c r="K108" s="48" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="109" spans="11:11">
-      <c r="K109" s="48" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="110" spans="11:11">
-      <c r="K110" s="48" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="111" spans="11:11">
-      <c r="K111" s="48" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="112" spans="11:11">
-      <c r="K112" s="48" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="113" spans="11:15">
-      <c r="K113" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="O113" s="8">
-        <v>40039</v>
-      </c>
-    </row>
-    <row r="114" spans="11:15">
-      <c r="K114" s="35" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="115" spans="11:15">
-      <c r="K115" s="35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="116" spans="11:15">
-      <c r="K116" s="35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="117" spans="11:15">
-      <c r="K117" s="35" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="118" spans="11:15">
-      <c r="K118" s="35" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="119" spans="11:15">
-      <c r="K119" s="35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="120" spans="11:15">
-      <c r="K120" s="35" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="121" spans="11:15">
-      <c r="K121" s="35" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="122" spans="11:15">
-      <c r="K122" s="35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="123" spans="11:15">
-      <c r="K123" s="35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="124" spans="11:15">
-      <c r="K124" s="35" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="125" spans="11:15">
-      <c r="K125" s="35" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="126" spans="11:15">
-      <c r="K126" s="35" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="127" spans="11:15">
-      <c r="K127" s="35" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="128" spans="11:15">
-      <c r="K128" s="35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="129" spans="11:11">
-      <c r="K129" s="35" t="s">
+    <row r="135" spans="15:15">
+      <c r="O135" s="35" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="130" spans="11:11">
-      <c r="K130" s="35" t="s">
+    <row r="136" spans="15:15">
+      <c r="O136" s="35" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="131" spans="11:11">
-      <c r="K131" s="35" t="s">
+    <row r="137" spans="15:15">
+      <c r="O137" s="35" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="132" spans="11:11">
-      <c r="K132" s="35" t="s">
+    <row r="138" spans="15:15">
+      <c r="O138" s="35" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="133" spans="11:11">
-      <c r="K133" s="35" t="s">
+    <row r="139" spans="15:15">
+      <c r="O139" s="35" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="134" spans="11:11">
-      <c r="K134" s="35" t="s">
+    <row r="140" spans="15:15">
+      <c r="O140" s="35" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="135" spans="11:11">
-      <c r="K135" s="35" t="s">
+    <row r="141" spans="15:15">
+      <c r="O141" s="35" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="136" spans="11:11">
-      <c r="K136" s="35" t="s">
+    <row r="142" spans="15:15">
+      <c r="O142" s="35" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="137" spans="11:11">
-      <c r="K137" s="35" t="s">
+    <row r="143" spans="15:15">
+      <c r="O143" s="35" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="138" spans="11:11">
-      <c r="K138" s="35" t="s">
+    <row r="144" spans="15:15">
+      <c r="O144" s="35" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="139" spans="11:11">
-      <c r="K139" s="35" t="s">
+    <row r="146" spans="15:16">
+      <c r="O146" s="51" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="140" spans="11:11">
-      <c r="K140" s="35" t="s">
+    <row r="147" spans="15:16">
+      <c r="O147" s="47" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="141" spans="11:11">
-      <c r="K141" s="35" t="s">
+    <row r="148" spans="15:16">
+      <c r="O148" s="47" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="142" spans="11:11">
-      <c r="K142" s="35" t="s">
+    <row r="149" spans="15:16">
+      <c r="O149" s="47" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="143" spans="11:11">
-      <c r="K143" s="35" t="s">
+    <row r="150" spans="15:16">
+      <c r="O150" s="47" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="144" spans="11:11">
-      <c r="K144" s="35" t="s">
+    <row r="151" spans="15:16">
+      <c r="O151" s="47" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="146" spans="11:11">
-      <c r="K146" s="53" t="s">
+      <c r="P151" s="11">
+        <v>40192</v>
+      </c>
+    </row>
+    <row r="152" spans="15:16">
+      <c r="O152" s="35" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="148" spans="11:11">
-      <c r="K148" s="35" t="s">
+    <row r="153" spans="15:16">
+      <c r="O153" s="35" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="150" spans="11:11">
-      <c r="K150" s="35" t="s">
+    <row r="154" spans="15:16">
+      <c r="O154" s="35" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="152" spans="11:11">
-      <c r="K152" s="35" t="s">
+    <row r="155" spans="15:16">
+      <c r="O155" s="35" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="154" spans="11:11">
-      <c r="K154" s="35" t="s">
+    <row r="156" spans="15:16">
+      <c r="O156" s="35" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="156" spans="11:11">
-      <c r="K156" s="35" t="s">
+    <row r="157" spans="15:16">
+      <c r="O157" s="35" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="158" spans="11:11">
-      <c r="K158" s="35" t="s">
+    <row r="158" spans="15:16">
+      <c r="O158" s="35" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="160" spans="11:11">
-      <c r="K160" s="35" t="s">
+    <row r="159" spans="15:16">
+      <c r="O159" s="35" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="162" spans="11:11">
-      <c r="K162" s="35" t="s">
+    <row r="160" spans="15:16">
+      <c r="O160" s="35" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="164" spans="11:11">
-      <c r="K164" s="35" t="s">
+    <row r="161" spans="15:16">
+      <c r="O161" s="35" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="166" spans="11:11">
-      <c r="K166" s="35" t="s">
+    <row r="162" spans="15:16">
+      <c r="O162" s="35" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="168" spans="11:11">
-      <c r="K168" s="35" t="s">
+    <row r="163" spans="15:16">
+      <c r="O163" s="35" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="170" spans="11:11">
-      <c r="K170" s="35" t="s">
+    <row r="165" spans="15:16">
+      <c r="O165" s="47" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="172" spans="11:11">
-      <c r="K172" s="35" t="s">
+    <row r="166" spans="15:16">
+      <c r="O166" s="47" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="174" spans="11:11">
-      <c r="K174" s="35" t="s">
+      <c r="P166" s="22">
+        <v>40618</v>
+      </c>
+    </row>
+    <row r="167" spans="15:16">
+      <c r="O167" s="35" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="176" spans="11:11">
-      <c r="K176" s="35" t="s">
+    <row r="168" spans="15:16">
+      <c r="O168" s="35" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="178" spans="11:11">
-      <c r="K178" s="35" t="s">
+    <row r="169" spans="15:16">
+      <c r="O169" s="35" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="180" spans="11:11">
-      <c r="K180" s="35" t="s">
+    <row r="170" spans="15:16">
+      <c r="O170" s="35" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="182" spans="11:11">
-      <c r="K182" s="35" t="s">
+    <row r="171" spans="15:16">
+      <c r="O171" s="35" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="184" spans="11:11">
-      <c r="K184" s="35" t="s">
+    <row r="172" spans="15:16">
+      <c r="O172" s="35" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="186" spans="11:11">
-      <c r="K186" s="35" t="s">
+    <row r="173" spans="15:16">
+      <c r="O173" s="35" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="188" spans="11:11">
-      <c r="K188" s="35" t="s">
+    <row r="174" spans="15:16">
+      <c r="O174" s="35" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="190" spans="11:11">
-      <c r="K190" s="35" t="s">
+    <row r="175" spans="15:16">
+      <c r="O175" s="35" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="192" spans="11:11">
-      <c r="K192" s="35" t="s">
+    <row r="176" spans="15:16">
+      <c r="O176" s="35" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="194" spans="11:11">
-      <c r="K194" s="35" t="s">
+    <row r="177" spans="15:16">
+      <c r="O177" s="35" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="196" spans="11:11">
-      <c r="K196" s="35" t="s">
+    <row r="179" spans="15:16">
+      <c r="O179" s="47" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="198" spans="11:11">
-      <c r="K198" s="35" t="s">
+    <row r="180" spans="15:16">
+      <c r="O180" s="47" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="200" spans="11:11">
-      <c r="K200" s="35" t="s">
+    <row r="181" spans="15:16">
+      <c r="O181" s="47" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="202" spans="11:11">
-      <c r="K202" s="35" t="s">
+    <row r="182" spans="15:16">
+      <c r="O182" s="47" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="204" spans="11:11">
-      <c r="K204" s="35" t="s">
+      <c r="P182" s="22">
+        <v>40659</v>
+      </c>
+    </row>
+    <row r="183" spans="15:16">
+      <c r="O183" s="35" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="206" spans="11:11">
-      <c r="K206" s="35" t="s">
+    <row r="184" spans="15:16">
+      <c r="O184" s="35" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="208" spans="11:11">
-      <c r="K208" s="35" t="s">
+    <row r="185" spans="15:16">
+      <c r="O185" s="35" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="210" spans="11:11">
-      <c r="K210" s="35" t="s">
+    <row r="186" spans="15:16">
+      <c r="O186" s="35" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="212" spans="11:11">
-      <c r="K212" s="35" t="s">
+    <row r="187" spans="15:16">
+      <c r="O187" s="35" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="214" spans="11:11">
-      <c r="K214" s="35" t="s">
+    <row r="188" spans="15:16">
+      <c r="O188" s="35" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="216" spans="11:11">
-      <c r="K216" s="35" t="s">
+    <row r="189" spans="15:16">
+      <c r="O189" s="35" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="218" spans="11:11">
-      <c r="K218" s="35" t="s">
+    <row r="190" spans="15:16">
+      <c r="O190" s="35" t="s">
         <v>274</v>
-      </c>
-    </row>
-    <row r="220" spans="11:11">
-      <c r="K220" s="35" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="222" spans="11:11">
-      <c r="K222" s="35" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="224" spans="11:11">
-      <c r="K224" s="35" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="226" spans="11:11">
-      <c r="K226" s="35" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="228" spans="11:11">
-      <c r="K228" s="35" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="230" spans="11:11">
-      <c r="K230" s="35" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="232" spans="11:11">
-      <c r="K232" s="35" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="234" spans="11:11">
-      <c r="K234" s="35" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="236" spans="11:11">
-      <c r="K236" s="35" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="238" spans="11:11">
-      <c r="K238" s="35" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="240" spans="11:11">
-      <c r="K240" s="35" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="242" spans="11:11">
-      <c r="K242" s="35" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="244" spans="11:11">
-      <c r="K244" s="35" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="246" spans="11:11">
-      <c r="K246" s="35" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="248" spans="11:11">
-      <c r="K248" s="35" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="250" spans="11:11">
-      <c r="K250" s="35" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="252" spans="11:11">
-      <c r="K252" s="35" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="254" spans="11:11">
-      <c r="K254" s="35" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="256" spans="11:11">
-      <c r="K256" s="35" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="258" spans="11:11">
-      <c r="K258" s="35" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="260" spans="11:11">
-      <c r="K260" s="35" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="262" spans="11:11">
-      <c r="K262" s="35" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="264" spans="11:11">
-      <c r="K264" s="35" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="266" spans="11:11">
-      <c r="K266" s="35" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="268" spans="11:11">
-      <c r="K268" s="35" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="270" spans="11:11">
-      <c r="K270" s="35" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="272" spans="11:11">
-      <c r="K272" s="35" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="274" spans="11:11">
-      <c r="K274" s="35" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="276" spans="11:11">
-      <c r="K276" s="35" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="278" spans="11:11">
-      <c r="K278" s="35" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="280" spans="11:11">
-      <c r="K280" s="35" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="282" spans="11:11">
-      <c r="K282" s="35" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="284" spans="11:11">
-      <c r="K284" s="35" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="286" spans="11:11">
-      <c r="K286" s="35" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="288" spans="11:11">
-      <c r="K288" s="35" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="290" spans="11:11">
-      <c r="K290" s="35" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="292" spans="11:11">
-      <c r="K292" s="35" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="294" spans="11:11">
-      <c r="K294" s="35" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="296" spans="11:11">
-      <c r="K296" s="35" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="298" spans="11:11">
-      <c r="K298" s="35" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="300" spans="11:11">
-      <c r="K300" s="35" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="302" spans="11:11">
-      <c r="K302" s="35" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="304" spans="11:11">
-      <c r="K304" s="35" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="306" spans="11:11">
-      <c r="K306" s="35" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="308" spans="11:11">
-      <c r="K308" s="35" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="310" spans="11:11">
-      <c r="K310" s="35" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="312" spans="11:11">
-      <c r="K312" s="35" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="314" spans="11:11">
-      <c r="K314" s="35" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="316" spans="11:11">
-      <c r="K316" s="35" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="318" spans="11:11">
-      <c r="K318" s="35" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="320" spans="11:11">
-      <c r="K320" s="35" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="322" spans="11:11">
-      <c r="K322" s="35" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="324" spans="11:11">
-      <c r="K324" s="35" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="326" spans="11:11">
-      <c r="K326" s="35" t="s">
-        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated spreadsheet and pop spike jpgs
</commit_message>
<xml_diff>
--- a/Documents/Dichter-data.xlsx
+++ b/Documents/Dichter-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="24280" windowWidth="25600" windowHeight="16060" activeTab="1"/>
+    <workbookView xWindow="6780" yWindow="24440" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original Dichter data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="119">
   <si>
     <t>Rat</t>
   </si>
@@ -367,7 +367,16 @@
     <t>I032_A0016</t>
   </si>
   <si>
-    <t>ch 3 &amp; 4 not used?</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>LCA1 &amp; LDG only</t>
+  </si>
+  <si>
+    <t>Seizure-like discharges?</t>
+  </si>
+  <si>
+    <t>don't use data after day 49</t>
   </si>
 </sst>
 </file>
@@ -377,7 +386,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -428,6 +437,11 @@
     <font>
       <sz val="13"/>
       <color theme="5" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -516,7 +530,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="229">
+  <cellStyleXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -746,8 +760,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -844,8 +872,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -880,13 +906,22 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="229">
+  <cellStyles count="243">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1001,6 +1036,13 @@
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1115,6 +1157,13 @@
     <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1417,10 +1466,10 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4:H48"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2511,1510 +2560,1089 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N70"/>
+  <dimension ref="A2:N72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="35" customWidth="1"/>
-    <col min="2" max="3" width="15.83203125" style="35" customWidth="1"/>
-    <col min="4" max="4" width="8" style="35" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" style="35" customWidth="1"/>
-    <col min="6" max="8" width="10.83203125" style="35"/>
-    <col min="9" max="9" width="16.6640625" style="35" customWidth="1"/>
-    <col min="10" max="11" width="15.83203125" style="35" customWidth="1"/>
-    <col min="12" max="14" width="10.83203125" style="35"/>
-    <col min="15" max="16" width="20" style="35" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="35"/>
+    <col min="1" max="1" width="6.33203125" style="35" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="35"/>
+    <col min="5" max="5" width="13.6640625" style="35" customWidth="1"/>
+    <col min="6" max="7" width="15.83203125" style="35" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="35"/>
+    <col min="10" max="10" width="14.5" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="35"/>
+    <col min="12" max="13" width="20" style="35" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="35"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="13" thickBot="1"/>
-    <row r="3" spans="1:13" ht="49" thickBot="1">
-      <c r="A3" s="45" t="s">
+    <row r="2" spans="1:14" ht="13" thickBot="1"/>
+    <row r="3" spans="1:14" ht="49" thickBot="1">
+      <c r="A3" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="M3" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="N3" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="50" t="s">
-        <v>99</v>
-      </c>
-      <c r="I3" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="J3" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="K3" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="L3" s="57" t="s">
-        <v>102</v>
-      </c>
-      <c r="M3" s="41" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="13" thickBot="1">
-      <c r="A4" s="36" t="s">
+    </row>
+    <row r="4" spans="1:14" ht="13" thickBot="1">
+      <c r="A4" s="18">
+        <v>1</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="49">
+        <v>65</v>
+      </c>
+      <c r="E4" s="50">
+        <v>7</v>
+      </c>
+      <c r="F4" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="M4" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="N4" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="18">
-        <v>1</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" s="51">
+    </row>
+    <row r="5" spans="1:14" ht="13" thickBot="1">
+      <c r="A5" s="35">
+        <v>2</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="49">
+        <v>56</v>
+      </c>
+      <c r="E5" s="50">
+        <v>10</v>
+      </c>
+      <c r="F5" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="L5" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="N5" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="35">
+        <v>3</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="51">
+        <v>53</v>
+      </c>
+      <c r="E6" s="52">
+        <v>7</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="L6" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="N6" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="38">
+        <v>4</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="51">
+        <v>56</v>
+      </c>
+      <c r="E7" s="52">
+        <v>25</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="38">
+        <v>5</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="51">
+        <v>203</v>
+      </c>
+      <c r="E8" s="53">
+        <v>8</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="M8" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8" s="35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="38">
+        <v>6</v>
+      </c>
+      <c r="B9" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="51">
+        <v>49</v>
+      </c>
+      <c r="E9" s="52">
+        <v>14</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="L9" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="M9" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="38">
+        <v>7</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="51">
+        <v>39</v>
+      </c>
+      <c r="E10" s="50">
+        <v>7</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="H10" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="M10" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" s="39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="38">
+        <v>8</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="51">
+        <v>130</v>
+      </c>
+      <c r="E11" s="52">
+        <v>36</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="N11" s="39"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="38">
+        <v>9</v>
+      </c>
+      <c r="B12" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="52">
-        <v>7</v>
-      </c>
-      <c r="J4" s="46" t="s">
+      <c r="C12" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="51">
+        <v>159</v>
+      </c>
+      <c r="E12" s="50">
+        <v>24</v>
+      </c>
+      <c r="F12" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="G12" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="H12" s="42" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="13" thickBot="1">
-      <c r="A5" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="35">
-        <v>2</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="51">
+      <c r="L12" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="N12" s="39"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="38">
+        <v>10</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="51">
+        <v>91</v>
+      </c>
+      <c r="E13" s="52">
+        <v>24</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" s="39"/>
+      <c r="N13" s="39"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="38">
+        <v>11</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="51">
+        <v>184</v>
+      </c>
+      <c r="E14" s="53">
+        <v>35</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="H14" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="N14" s="39"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="38">
+        <v>12</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="51">
+        <v>63</v>
+      </c>
+      <c r="E15" s="53">
+        <v>14</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="J15" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" s="37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="38">
+        <v>13</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="54">
+        <v>51</v>
+      </c>
+      <c r="E16" s="53">
+        <v>14</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="42"/>
+      <c r="J16" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="L16" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="52">
-        <v>10</v>
-      </c>
-      <c r="J5" s="46" t="s">
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="38">
+        <v>14</v>
+      </c>
+      <c r="B17" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="51">
+        <v>98</v>
+      </c>
+      <c r="E17" s="52">
+        <v>8</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="H17" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" s="35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="38">
+        <v>15</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="51">
+        <v>49</v>
+      </c>
+      <c r="E18" s="56">
+        <v>14</v>
+      </c>
+      <c r="F18" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="G18" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="L5" s="35" t="s">
+      <c r="H18" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="M5" s="35" t="s">
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="38">
+        <v>16</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="51">
+        <v>52</v>
+      </c>
+      <c r="F19" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="38" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="35">
-        <v>3</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" s="53">
-        <v>53</v>
-      </c>
-      <c r="I6" s="54">
-        <v>7</v>
-      </c>
-      <c r="J6" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" s="38" t="s">
+      <c r="H19" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="L6" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="M6" s="44" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="38">
-        <v>4</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="H7" s="53">
-        <v>56</v>
-      </c>
-      <c r="I7" s="54">
-        <v>25</v>
-      </c>
-      <c r="J7" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="K7" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="L7" s="38" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="38">
-        <v>5</v>
-      </c>
-      <c r="F8" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="G8" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="53">
-        <v>203</v>
-      </c>
-      <c r="I8" s="55">
-        <v>8</v>
-      </c>
-      <c r="J8" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="38">
-        <v>6</v>
-      </c>
-      <c r="F9" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" s="53">
-        <v>49</v>
-      </c>
-      <c r="I9" s="54">
-        <v>14</v>
-      </c>
-      <c r="J9" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="K9" s="38" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="C10" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="38">
-        <v>7</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="H10" s="53">
-        <v>39</v>
-      </c>
-      <c r="I10" s="52">
-        <v>7</v>
-      </c>
-      <c r="J10" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="K10" s="44" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="39"/>
-      <c r="C11" s="58" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="38">
-        <v>8</v>
-      </c>
-      <c r="F11" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" s="53">
-        <v>130</v>
-      </c>
-      <c r="I11" s="54">
-        <v>36</v>
-      </c>
-      <c r="J11" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="K11" s="44"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="C12" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="38">
-        <v>9</v>
-      </c>
-      <c r="F12" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="H12" s="53">
-        <v>159</v>
-      </c>
-      <c r="I12" s="52">
-        <v>24</v>
-      </c>
-      <c r="J12" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="K12" s="43"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="38">
-        <v>10</v>
-      </c>
-      <c r="F13" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="H13" s="53">
-        <v>91</v>
-      </c>
-      <c r="I13" s="54">
-        <v>24</v>
-      </c>
-      <c r="J13" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" s="44"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="38">
-        <v>11</v>
-      </c>
-      <c r="F14" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="53">
-        <v>184</v>
-      </c>
-      <c r="I14" s="55">
-        <v>35</v>
-      </c>
-      <c r="J14" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="K14" s="44"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="C15" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="38">
-        <v>12</v>
-      </c>
-      <c r="F15" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="H15" s="53">
-        <v>63</v>
-      </c>
-      <c r="I15" s="55">
-        <v>14</v>
-      </c>
-      <c r="J15" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="K15" s="44" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="E16" s="38">
-        <v>13</v>
-      </c>
-      <c r="F16" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" t="s">
-        <v>111</v>
-      </c>
-      <c r="H16" s="56">
-        <v>51</v>
-      </c>
-      <c r="I16" s="55">
-        <v>14</v>
-      </c>
-      <c r="J16" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="K16" s="44" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="E17" s="38">
-        <v>14</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H17" s="53">
-        <v>98</v>
-      </c>
-      <c r="I17" s="54">
-        <v>8</v>
-      </c>
-      <c r="J17" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="K17" s="44"/>
-    </row>
-    <row r="18" spans="1:14">
-      <c r="E18" s="38">
-        <v>15</v>
-      </c>
-      <c r="F18" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="G18" t="s">
-        <v>113</v>
-      </c>
-      <c r="H18" s="53">
-        <v>49</v>
-      </c>
-      <c r="I18" s="60">
-        <v>14</v>
-      </c>
-      <c r="J18" s="47" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="E19" s="38">
-        <v>16</v>
-      </c>
-      <c r="F19" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="G19" t="s">
-        <v>114</v>
-      </c>
-      <c r="J19" s="38" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="N21" s="48"/>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="N22" s="49"/>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="N23" s="48"/>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="7">
-        <v>97</v>
-      </c>
-      <c r="B24" s="8">
-        <v>39512</v>
-      </c>
-      <c r="C24" s="8">
-        <v>39519</v>
-      </c>
-      <c r="D24" s="8">
-        <v>39577</v>
-      </c>
-      <c r="E24" s="9">
-        <f>D24-B24</f>
-        <v>65</v>
-      </c>
-      <c r="F24" s="9">
-        <f>C24-B24</f>
-        <v>7</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="N24" s="49"/>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="1"/>
-      <c r="N25" s="48"/>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="7">
-        <v>99</v>
-      </c>
-      <c r="B26" s="8">
-        <v>39577</v>
-      </c>
-      <c r="C26" s="8">
-        <v>39587</v>
-      </c>
-      <c r="D26" s="8">
-        <v>39633</v>
-      </c>
-      <c r="E26" s="9">
-        <f>D26-B26</f>
-        <v>56</v>
-      </c>
-      <c r="F26" s="9">
-        <f>C26-B26</f>
-        <v>10</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="49"/>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="1"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="48"/>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28">
-        <v>100</v>
-      </c>
-      <c r="B28" s="11">
-        <v>39590</v>
-      </c>
-      <c r="C28" s="11">
-        <v>39597</v>
-      </c>
-      <c r="D28" s="11">
-        <v>39643</v>
-      </c>
-      <c r="E28" s="2">
-        <f>D28-B28</f>
-        <v>53</v>
-      </c>
-      <c r="F28" s="2">
-        <f>C28-B28</f>
-        <v>7</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="49"/>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="1"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="48"/>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30">
-        <v>101</v>
-      </c>
-      <c r="B30" s="11">
-        <v>39604</v>
-      </c>
-      <c r="C30" s="11">
-        <v>39629</v>
-      </c>
-      <c r="D30" s="11">
-        <v>39660</v>
-      </c>
-      <c r="E30" s="2">
-        <f>D30-B30</f>
-        <v>56</v>
-      </c>
-      <c r="F30" s="2">
-        <f>C30-B30</f>
-        <v>25</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="49"/>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="1"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="48"/>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32">
-        <v>103</v>
-      </c>
-      <c r="B32" s="11">
-        <v>39660</v>
-      </c>
-      <c r="C32" s="11">
-        <v>39675</v>
-      </c>
-      <c r="D32" s="11">
-        <v>39675</v>
-      </c>
-      <c r="E32" s="2">
-        <f>D32-B32</f>
-        <v>15</v>
-      </c>
-      <c r="F32" s="2">
-        <f>C32-B32</f>
-        <v>15</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="49"/>
-    </row>
-    <row r="33" spans="1:14">
-      <c r="A33"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="1"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="48"/>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="A34" s="7">
-        <v>104</v>
-      </c>
-      <c r="B34" s="8">
-        <v>39667</v>
-      </c>
-      <c r="C34" s="8">
-        <v>39675</v>
-      </c>
-      <c r="D34" s="8">
-        <v>39870</v>
-      </c>
-      <c r="E34" s="9">
-        <f>D34-B34</f>
-        <v>203</v>
-      </c>
-      <c r="F34" s="9">
-        <f>C34-B34</f>
-        <v>8</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="49"/>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="A35"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="1"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="49"/>
-      <c r="N35" s="48"/>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36">
-        <v>107</v>
-      </c>
-      <c r="B36" s="11">
-        <v>39689</v>
-      </c>
-      <c r="C36" s="11">
-        <v>39703</v>
-      </c>
-      <c r="D36" s="11">
-        <v>39738</v>
-      </c>
-      <c r="E36" s="2">
-        <f>D36-B36</f>
-        <v>49</v>
-      </c>
-      <c r="F36" s="2">
-        <f>C36-B36</f>
-        <v>14</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="48"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="49"/>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="1"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="48"/>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38">
-        <v>118</v>
-      </c>
-      <c r="B38" s="11">
-        <v>39853</v>
-      </c>
-      <c r="C38" s="11">
-        <v>39871</v>
-      </c>
-      <c r="D38" s="11">
-        <v>401461</v>
-      </c>
-      <c r="E38" s="2">
-        <v>18</v>
-      </c>
-      <c r="F38" s="14">
-        <f>C38-B38</f>
-        <v>18</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="48"/>
-      <c r="M38" s="48"/>
-      <c r="N38" s="49"/>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="A39"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="1"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="48"/>
-    </row>
-    <row r="40" spans="1:14">
-      <c r="A40" s="7">
-        <v>121</v>
-      </c>
-      <c r="B40" s="8">
-        <v>39889</v>
-      </c>
-      <c r="C40" s="8">
-        <v>39896</v>
-      </c>
-      <c r="D40" s="8">
-        <v>39928</v>
-      </c>
-      <c r="E40" s="9">
-        <f>D40-B40</f>
-        <v>39</v>
-      </c>
-      <c r="F40" s="14">
-        <f>C40-B40</f>
-        <v>7</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="48"/>
-      <c r="M40" s="48"/>
-      <c r="N40" s="49"/>
-    </row>
-    <row r="41" spans="1:14">
-      <c r="A41"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="1"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="49"/>
-      <c r="M41" s="49"/>
-      <c r="N41" s="48"/>
-    </row>
-    <row r="42" spans="1:14">
-      <c r="A42">
-        <v>127</v>
-      </c>
-      <c r="B42" s="11">
-        <v>40000</v>
-      </c>
-      <c r="C42" s="11">
-        <v>40036</v>
-      </c>
-      <c r="D42" s="11">
-        <v>40130</v>
-      </c>
-      <c r="E42" s="14">
-        <f>D42-B42</f>
-        <v>130</v>
-      </c>
-      <c r="F42" s="14">
-        <f>C42-B42</f>
-        <v>36</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="48"/>
-      <c r="M42" s="48"/>
-      <c r="N42" s="49"/>
-    </row>
-    <row r="43" spans="1:14">
-      <c r="A43"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="1"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="49"/>
-      <c r="N43" s="48"/>
-    </row>
-    <row r="44" spans="1:14">
-      <c r="A44" s="7">
-        <v>130</v>
-      </c>
-      <c r="B44" s="8">
-        <v>40015</v>
-      </c>
-      <c r="C44" s="8">
-        <v>40039</v>
-      </c>
-      <c r="D44" s="8">
-        <v>40174</v>
-      </c>
-      <c r="E44" s="9">
-        <f>D44-B44</f>
-        <v>159</v>
-      </c>
-      <c r="F44" s="14">
-        <f>C44-B44</f>
-        <v>24</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="48"/>
-      <c r="M44" s="48"/>
-      <c r="N44" s="48"/>
-    </row>
-    <row r="45" spans="1:14">
-      <c r="A45"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="1"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="49"/>
-      <c r="M45" s="49"/>
-      <c r="N45" s="48"/>
-    </row>
-    <row r="46" spans="1:14">
-      <c r="A46">
-        <v>137</v>
-      </c>
-      <c r="B46" s="11">
-        <v>40168</v>
-      </c>
-      <c r="C46" s="11">
-        <v>40192</v>
-      </c>
-      <c r="D46" s="11">
-        <v>40259</v>
-      </c>
-      <c r="E46" s="14">
-        <f>D46-B46</f>
-        <v>91</v>
-      </c>
-      <c r="F46" s="14">
-        <f>C46-B46</f>
-        <v>24</v>
-      </c>
-      <c r="G46" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="48"/>
-      <c r="M46" s="48"/>
-      <c r="N46" s="49"/>
-    </row>
-    <row r="47" spans="1:14">
-      <c r="A47"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="20"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="49"/>
-      <c r="M47" s="49"/>
-      <c r="N47" s="48"/>
-    </row>
-    <row r="48" spans="1:14">
-      <c r="A48" s="21">
-        <v>146</v>
-      </c>
-      <c r="B48" s="22">
-        <v>40512</v>
-      </c>
-      <c r="C48" s="22">
-        <v>40547</v>
-      </c>
-      <c r="D48" s="22">
-        <v>40696</v>
-      </c>
-      <c r="E48" s="23">
-        <f>D48-B48</f>
-        <v>184</v>
-      </c>
-      <c r="F48" s="23">
-        <f>C48-B48</f>
-        <v>35</v>
-      </c>
-      <c r="G48" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="48"/>
-      <c r="M48" s="48"/>
-      <c r="N48" s="48"/>
-    </row>
-    <row r="49" spans="1:14">
-      <c r="A49"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="1"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="48"/>
-      <c r="M49" s="48"/>
-      <c r="N49" s="48"/>
-    </row>
-    <row r="50" spans="1:14">
-      <c r="A50" s="21">
-        <v>151</v>
-      </c>
-      <c r="B50" s="22">
-        <v>40604</v>
-      </c>
-      <c r="C50" s="22">
-        <v>40618</v>
-      </c>
-      <c r="D50" s="22">
-        <v>40667</v>
-      </c>
-      <c r="E50" s="23">
-        <f>D50-B50</f>
-        <v>63</v>
-      </c>
-      <c r="F50" s="23">
-        <f>C50-B50</f>
-        <v>14</v>
-      </c>
-      <c r="G50" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="48"/>
-      <c r="M50" s="48"/>
-      <c r="N50" s="49"/>
-    </row>
-    <row r="51" spans="1:14">
-      <c r="A51"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="1"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="49"/>
-      <c r="M51" s="49"/>
-      <c r="N51" s="48"/>
-    </row>
-    <row r="52" spans="1:14">
-      <c r="A52" s="21">
-        <v>152</v>
-      </c>
-      <c r="B52" s="22">
-        <v>40645</v>
-      </c>
-      <c r="C52" s="22">
-        <v>40659</v>
-      </c>
-      <c r="D52" s="22">
-        <v>40696</v>
-      </c>
-      <c r="E52" s="23">
-        <f>D52-B52</f>
-        <v>51</v>
-      </c>
-      <c r="F52" s="23">
-        <f>C52-B52</f>
-        <v>14</v>
-      </c>
-      <c r="G52" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="J52" s="18"/>
-      <c r="K52" s="18"/>
-      <c r="L52" s="48"/>
-      <c r="M52" s="48"/>
-      <c r="N52" s="49"/>
-    </row>
-    <row r="53" spans="1:14">
-      <c r="A53"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="1"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18"/>
-      <c r="L53" s="48"/>
-      <c r="M53" s="48"/>
-      <c r="N53" s="48"/>
-    </row>
-    <row r="54" spans="1:14">
-      <c r="A54" t="s">
-        <v>25</v>
-      </c>
-      <c r="B54" s="11">
-        <v>40680</v>
-      </c>
-      <c r="C54" s="11">
-        <v>40687</v>
-      </c>
-      <c r="D54" s="11">
-        <v>40700</v>
-      </c>
-      <c r="E54" s="14">
-        <f>D54-B54</f>
-        <v>20</v>
-      </c>
-      <c r="F54" s="14">
-        <f>C54-B54</f>
-        <v>7</v>
-      </c>
-      <c r="G54" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="48"/>
-      <c r="M54" s="48"/>
-      <c r="N54" s="49"/>
-    </row>
-    <row r="55" spans="1:14">
-      <c r="A55"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="1"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="49"/>
-      <c r="M55" s="49"/>
-      <c r="N55" s="48"/>
-    </row>
-    <row r="56" spans="1:14">
-      <c r="A56">
-        <v>157</v>
-      </c>
-      <c r="B56" s="11">
-        <v>40735</v>
-      </c>
-      <c r="C56" s="11">
-        <v>40743</v>
-      </c>
-      <c r="D56" s="11">
-        <v>40833</v>
-      </c>
-      <c r="E56" s="14">
-        <f>D56-B56</f>
-        <v>98</v>
-      </c>
-      <c r="F56" s="14">
-        <f>C56-B56</f>
-        <v>8</v>
-      </c>
-      <c r="G56" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
-      <c r="L56" s="48"/>
-      <c r="M56" s="48"/>
-      <c r="N56" s="48"/>
-    </row>
-    <row r="57" spans="1:14">
-      <c r="A57"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="1"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="49"/>
-      <c r="M57" s="49"/>
-      <c r="N57" s="48"/>
-    </row>
-    <row r="58" spans="1:14">
-      <c r="A58">
-        <v>158</v>
-      </c>
-      <c r="B58" s="11">
-        <v>40735</v>
-      </c>
-      <c r="C58" s="11">
-        <v>40743</v>
-      </c>
-      <c r="D58" s="11">
-        <v>40756</v>
-      </c>
-      <c r="E58" s="14">
-        <f>D58-B58</f>
-        <v>21</v>
-      </c>
-      <c r="F58" s="14">
-        <f>C58-B58</f>
-        <v>8</v>
-      </c>
-      <c r="G58" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="J58" s="18"/>
-      <c r="K58" s="18"/>
-      <c r="L58" s="48"/>
-      <c r="M58" s="48"/>
-      <c r="N58" s="49"/>
-    </row>
-    <row r="59" spans="1:14">
-      <c r="A59"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="1"/>
-      <c r="J59" s="18"/>
-      <c r="K59" s="18"/>
-      <c r="L59" s="49"/>
-      <c r="M59" s="49"/>
-      <c r="N59" s="48"/>
-    </row>
-    <row r="60" spans="1:14">
-      <c r="A60" s="21">
-        <v>161</v>
-      </c>
-      <c r="B60" s="22">
-        <v>40745</v>
-      </c>
-      <c r="C60" s="22">
-        <v>40759</v>
-      </c>
-      <c r="D60" s="22">
-        <v>40794</v>
-      </c>
-      <c r="E60" s="23">
-        <f>D60-B60</f>
-        <v>49</v>
-      </c>
-      <c r="F60" s="23">
-        <f>C60-B60</f>
-        <v>14</v>
-      </c>
-      <c r="G60" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="J60" s="18"/>
-      <c r="K60" s="18"/>
-      <c r="L60" s="48"/>
-      <c r="M60" s="48"/>
-      <c r="N60" s="49"/>
-    </row>
-    <row r="61" spans="1:14">
-      <c r="A61"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="1"/>
-      <c r="J61" s="18"/>
-      <c r="K61" s="18"/>
-      <c r="L61" s="48"/>
-      <c r="M61" s="48"/>
-      <c r="N61" s="48"/>
-    </row>
-    <row r="62" spans="1:14">
-      <c r="A62">
-        <v>162</v>
-      </c>
-      <c r="B62" s="11">
-        <v>40752</v>
-      </c>
-      <c r="C62" s="11">
-        <v>40759</v>
-      </c>
-      <c r="D62" s="11">
-        <v>40778</v>
-      </c>
-      <c r="E62" s="14">
-        <f>D62-B62</f>
-        <v>26</v>
-      </c>
-      <c r="F62" s="14">
-        <f>C62-B62</f>
-        <v>7</v>
-      </c>
-      <c r="G62" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="J62" s="18"/>
-      <c r="K62" s="18"/>
-      <c r="L62" s="48"/>
-      <c r="M62" s="48"/>
-      <c r="N62" s="49"/>
-    </row>
-    <row r="63" spans="1:14">
-      <c r="A63"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="1"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="18"/>
-      <c r="L63" s="49"/>
-      <c r="M63" s="49"/>
-      <c r="N63" s="48"/>
-    </row>
-    <row r="64" spans="1:14">
-      <c r="A64">
-        <v>164</v>
-      </c>
-      <c r="B64" s="11">
-        <v>40778</v>
-      </c>
-      <c r="C64" s="11">
-        <v>40793</v>
-      </c>
-      <c r="D64" s="11">
-        <v>40799</v>
-      </c>
-      <c r="E64" s="14">
-        <f>D64-B64</f>
-        <v>21</v>
-      </c>
-      <c r="F64" s="14">
-        <f>C64-B64</f>
-        <v>15</v>
-      </c>
-      <c r="G64" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="J64" s="18"/>
-      <c r="K64" s="18"/>
-      <c r="L64" s="48"/>
-      <c r="M64" s="48"/>
-      <c r="N64" s="49"/>
-    </row>
-    <row r="65" spans="1:14">
-      <c r="A65"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="1"/>
-      <c r="J65" s="18"/>
-      <c r="K65" s="18"/>
-      <c r="L65" s="49"/>
-      <c r="M65" s="49"/>
-      <c r="N65" s="48"/>
-    </row>
-    <row r="66" spans="1:14">
-      <c r="A66" s="21">
-        <v>165</v>
-      </c>
-      <c r="B66" s="22">
-        <v>40774</v>
-      </c>
-      <c r="C66" s="22">
-        <v>40793</v>
-      </c>
-      <c r="D66" s="22">
-        <v>40857</v>
-      </c>
-      <c r="E66" s="23"/>
-      <c r="F66" s="23">
-        <f>C66-B66</f>
-        <v>19</v>
-      </c>
-      <c r="G66" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="J66" s="18"/>
-      <c r="K66" s="18"/>
-      <c r="L66" s="48"/>
-      <c r="M66" s="48"/>
-    </row>
-    <row r="67" spans="1:14">
-      <c r="A67"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="1"/>
-      <c r="J67" s="18"/>
-      <c r="K67" s="18"/>
-      <c r="L67" s="49"/>
-      <c r="M67" s="49"/>
-    </row>
-    <row r="68" spans="1:14">
-      <c r="A68">
-        <v>168</v>
-      </c>
-      <c r="B68" s="11">
-        <v>40792</v>
-      </c>
-      <c r="C68" s="11">
-        <v>40798</v>
-      </c>
-      <c r="D68" s="11">
-        <v>40843</v>
-      </c>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14">
-        <f>C68-B68</f>
-        <v>6</v>
-      </c>
-      <c r="G68" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="J68" s="18"/>
-      <c r="K68" s="18"/>
-      <c r="L68" s="48"/>
-      <c r="M68" s="48"/>
-    </row>
-    <row r="69" spans="1:14">
-      <c r="J69" s="18"/>
-      <c r="K69" s="18"/>
-      <c r="L69" s="49"/>
-      <c r="M69" s="49"/>
-    </row>
-    <row r="70" spans="1:14">
-      <c r="J70" s="18"/>
-      <c r="K70" s="18"/>
-      <c r="L70" s="48"/>
-      <c r="M70" s="48"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="K21" s="46"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="K22" s="47"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="K23" s="46"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="47"/>
+      <c r="K24" s="47"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="47"/>
+      <c r="K25" s="46"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="47"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="47"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="47"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="46"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="47"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="47"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="47"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="46"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="47"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="47"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="47"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="46"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="47"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="47"/>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="47"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="46"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="47"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="47"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="47"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="46"/>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="47"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="47"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="47"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="47"/>
+      <c r="J37" s="47"/>
+      <c r="K37" s="46"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="47"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="47"/>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="47"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="47"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="46"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="47"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="47"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="47"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="46"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="47"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="47"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="47"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="46"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="47"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
+      <c r="J44" s="46"/>
+      <c r="K44" s="46"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="14"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="47"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="46"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="47"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="47"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="47"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="47"/>
+      <c r="I47" s="47"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="46"/>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="47"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="46"/>
+      <c r="J48" s="46"/>
+      <c r="K48" s="46"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="47"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="46"/>
+      <c r="J49" s="46"/>
+      <c r="K49" s="46"/>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="47"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="47"/>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="47"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="47"/>
+      <c r="I51" s="47"/>
+      <c r="J51" s="47"/>
+      <c r="K51" s="46"/>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="47"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="46"/>
+      <c r="I52" s="46"/>
+      <c r="J52" s="46"/>
+      <c r="K52" s="47"/>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="47"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
+      <c r="J53" s="46"/>
+      <c r="K53" s="46"/>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="61"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="47"/>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="47"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="47"/>
+      <c r="I55" s="47"/>
+      <c r="J55" s="47"/>
+      <c r="K55" s="46"/>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="61"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="46"/>
+      <c r="I56" s="46"/>
+      <c r="J56" s="46"/>
+      <c r="K56" s="46"/>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="47"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="47"/>
+      <c r="J57" s="47"/>
+      <c r="K57" s="46"/>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="61"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
+      <c r="J58" s="46"/>
+      <c r="K58" s="47"/>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="14"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="47"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="47"/>
+      <c r="J59" s="47"/>
+      <c r="K59" s="46"/>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="14"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="47"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="46"/>
+      <c r="I60" s="46"/>
+      <c r="J60" s="46"/>
+      <c r="K60" s="47"/>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="14"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="47"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="46"/>
+      <c r="I61" s="46"/>
+      <c r="J61" s="46"/>
+      <c r="K61" s="46"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="61"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="46"/>
+      <c r="I62" s="46"/>
+      <c r="J62" s="46"/>
+      <c r="K62" s="47"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="47"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="47"/>
+      <c r="I63" s="47"/>
+      <c r="J63" s="47"/>
+      <c r="K63" s="46"/>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="61"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="46"/>
+      <c r="I64" s="46"/>
+      <c r="J64" s="46"/>
+      <c r="K64" s="47"/>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="47"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="47"/>
+      <c r="I65" s="47"/>
+      <c r="J65" s="47"/>
+      <c r="K65" s="46"/>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="47"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="46"/>
+      <c r="I66" s="46"/>
+      <c r="J66" s="46"/>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="14"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="47"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="47"/>
+      <c r="I67" s="47"/>
+      <c r="J67" s="47"/>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="47"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="46"/>
+      <c r="I68" s="46"/>
+      <c r="J68" s="46"/>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="58"/>
+      <c r="B69" s="58"/>
+      <c r="C69" s="58"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="47"/>
+      <c r="I69" s="47"/>
+      <c r="J69" s="47"/>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="58"/>
+      <c r="B70" s="58"/>
+      <c r="C70" s="58"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="46"/>
+      <c r="I70" s="46"/>
+      <c r="J70" s="46"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="58"/>
+      <c r="B71" s="58"/>
+      <c r="C71" s="58"/>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="58"/>
+      <c r="B72" s="58"/>
+      <c r="C72" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Deleted extra lines from f_eeg2mef
</commit_message>
<xml_diff>
--- a/Documents/Dichter-data.xlsx
+++ b/Documents/Dichter-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="24440" windowWidth="25600" windowHeight="16060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original Dichter data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="119">
   <si>
     <t>Rat</t>
   </si>
@@ -367,16 +367,16 @@
     <t>I032_A0016</t>
   </si>
   <si>
+    <t>LCA1 &amp; LDG only</t>
+  </si>
+  <si>
+    <t>Seizure-like discharges?</t>
+  </si>
+  <si>
+    <t>don't use data after day 49</t>
+  </si>
+  <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>LCA1 &amp; LDG only</t>
-  </si>
-  <si>
-    <t>Seizure-like discharges?</t>
-  </si>
-  <si>
-    <t>don't use data after day 49</t>
   </si>
 </sst>
 </file>
@@ -2563,7 +2563,7 @@
   <dimension ref="A2:N72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2681,6 +2681,9 @@
       <c r="H5" s="35" t="s">
         <v>98</v>
       </c>
+      <c r="I5" s="57" t="s">
+        <v>118</v>
+      </c>
       <c r="L5" s="36" t="s">
         <v>83</v>
       </c>
@@ -2716,7 +2719,9 @@
       <c r="H6" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="42" t="s">
+        <v>118</v>
+      </c>
       <c r="J6" s="42"/>
       <c r="L6" s="58" t="s">
         <v>84</v>
@@ -2824,7 +2829,7 @@
         <v>98</v>
       </c>
       <c r="J9" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L9" s="59" t="s">
         <v>87</v>
@@ -2979,10 +2984,10 @@
         <v>95</v>
       </c>
       <c r="G14" s="42" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="H14" s="57" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="N14" s="39"/>
     </row>
@@ -3012,7 +3017,7 @@
         <v>98</v>
       </c>
       <c r="J15" s="35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L15" s="37" t="s">
         <v>55</v>
@@ -3037,9 +3042,14 @@
       <c r="F16" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="G16" s="42"/>
+      <c r="G16" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="57" t="s">
+        <v>98</v>
+      </c>
       <c r="J16" s="35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L16" s="37" t="s">
         <v>56</v>
@@ -3071,7 +3081,7 @@
         <v>98</v>
       </c>
       <c r="J17" s="35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:11">

</xml_diff>